<commit_message>
done till update the file
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -2734,7 +2734,11 @@
         </is>
       </c>
       <c r="X10" s="16" t="inlineStr"/>
-      <c r="Y10" s="16" t="n"/>
+      <c r="Y10" s="16" t="inlineStr">
+        <is>
+          <t>2023-01-16 16:44:28 (bot) : Updated by bot at this time</t>
+        </is>
+      </c>
       <c r="Z10" s="20" t="inlineStr">
         <is>
           <t>Installed</t>

</xml_diff>

<commit_message>
able to update for all parameters
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -2673,7 +2673,7 @@
       </c>
       <c r="F10" s="22" t="inlineStr">
         <is>
-          <t>https://docs.fortinet.com/document/fortigate/7.0.9/fortios-release-notes/553516/change-log</t>
+          <t>https://support.fortinet.com/Information/ProductLifeCycle.aspx</t>
         </is>
       </c>
       <c r="G10" s="17" t="n">
@@ -2697,13 +2697,11 @@
       </c>
       <c r="L10" s="16" t="inlineStr">
         <is>
-          <t>7.0.9</t>
-        </is>
-      </c>
-      <c r="M10" s="17" t="inlineStr">
-        <is>
-          <t>2022-11-22</t>
-        </is>
+          <t>7.0.8</t>
+        </is>
+      </c>
+      <c r="M10" s="17" t="n">
+        <v>44847</v>
       </c>
       <c r="N10" s="17" t="n">
         <v>44847</v>
@@ -2742,11 +2740,6 @@
       <c r="Z10" s="20" t="inlineStr">
         <is>
           <t>Installed</t>
-        </is>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>2023-01-17 17:12:55 (bot) : Updated by bot at this time</t>
         </is>
       </c>
     </row>
@@ -2992,7 +2985,7 @@
       </c>
       <c r="F13" s="22" t="inlineStr">
         <is>
-          <t>https://support.fortinet.com/Information/ProductLifeCycle.aspx</t>
+          <t>https://docs.fortinet.com/document/fortimanager/7.0.5/release-notes/441895/change-log</t>
         </is>
       </c>
       <c r="G13" s="9" t="n">
@@ -3019,8 +3012,10 @@
           <t>7.0.5</t>
         </is>
       </c>
-      <c r="M13" s="17" t="n">
-        <v>44847</v>
+      <c r="M13" s="17" t="inlineStr">
+        <is>
+          <t>2022-10-13</t>
+        </is>
       </c>
       <c r="N13" s="17" t="n">
         <v>44847</v>
@@ -3068,6 +3063,11 @@
       <c r="Z13" s="10" t="inlineStr">
         <is>
           <t>Installed</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>2023-01-30 19:25:55 (bot) : Updated by bot at this time</t>
         </is>
       </c>
     </row>

</xml_diff>